<commit_message>
Minor bug fixes with adding modifiers and deleting columns.
Set up multi-permissive admin system.
Customers can no longer delete items.
Prices auto format to dollar notation.
</commit_message>
<xml_diff>
--- a/src/static/exports/Hummels Demo.xlsx
+++ b/src/static/exports/Hummels Demo.xlsx
@@ -17,15 +17,16 @@
     <sheet name="Kitchen Food" sheetId="8" r:id="rId8"/>
     <sheet name="Bar Snacks" sheetId="9" r:id="rId9"/>
     <sheet name="Merchandise" sheetId="10" r:id="rId10"/>
-    <sheet name="Paids" sheetId="11" r:id="rId11"/>
-    <sheet name="Employees" sheetId="12" r:id="rId12"/>
+    <sheet name="test" sheetId="11" r:id="rId11"/>
+    <sheet name="Paids" sheetId="12" r:id="rId12"/>
+    <sheet name="Employees" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="223">
   <si>
     <t xml:space="preserve">Items: </t>
   </si>
@@ -57,10 +58,7 @@
     <t>Troegs IPA</t>
   </si>
   <si>
-    <t>Truly</t>
-  </si>
-  <si>
-    <t>Twisted Tea</t>
+    <t>test</t>
   </si>
   <si>
     <t>Arnold Palmer</t>
@@ -355,9 +353,6 @@
   </si>
   <si>
     <t>Pickle Shot</t>
-  </si>
-  <si>
-    <t>Trash Can</t>
   </si>
   <si>
     <t>White Russian</t>
@@ -663,7 +658,7 @@
     <t>Amanda P</t>
   </si>
   <si>
-    <t>0120</t>
+    <t>1234</t>
   </si>
   <si>
     <t>Manager</t>
@@ -672,67 +667,37 @@
     <t>Candace S</t>
   </si>
   <si>
-    <t>0350</t>
-  </si>
-  <si>
     <t>Beth S</t>
   </si>
   <si>
-    <t>9584</t>
-  </si>
-  <si>
     <t>Cook</t>
   </si>
   <si>
     <t>Joanne S</t>
   </si>
   <si>
-    <t>0153</t>
-  </si>
-  <si>
     <t>Bartender</t>
   </si>
   <si>
     <t>Kristin P</t>
   </si>
   <si>
-    <t>2692</t>
-  </si>
-  <si>
     <t>Maryann K</t>
   </si>
   <si>
-    <t>4718</t>
-  </si>
-  <si>
     <t>Monica C</t>
   </si>
   <si>
-    <t>5895</t>
-  </si>
-  <si>
     <t>Morgan S</t>
   </si>
   <si>
-    <t>3131</t>
-  </si>
-  <si>
     <t>Renee A</t>
   </si>
   <si>
-    <t>0531</t>
-  </si>
-  <si>
     <t>Roxane A</t>
   </si>
   <si>
-    <t>0123</t>
-  </si>
-  <si>
     <t>Colleen P</t>
-  </si>
-  <si>
-    <t>0036</t>
   </si>
 </sst>
 </file>
@@ -1064,7 +1029,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1097,23 +1062,12 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
         <v>10</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1145,7 +1099,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B2">
         <v>1.75</v>
@@ -1153,7 +1107,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B3">
         <v>0.25</v>
@@ -1165,6 +1119,33 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D8"/>
   <sheetViews>
@@ -1174,48 +1155,48 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -1223,7 +1204,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C12"/>
   <sheetViews>
@@ -1233,134 +1214,134 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C1" t="s">
         <v>207</v>
-      </c>
-      <c r="B1" t="s">
-        <v>208</v>
-      </c>
-      <c r="C1" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C2" t="s">
         <v>210</v>
-      </c>
-      <c r="B2" t="s">
-        <v>211</v>
-      </c>
-      <c r="C2" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B3" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="C3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B4" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="C4" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B5" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="C5" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B6" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
       <c r="C6" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="B7" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="C7" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="B8" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="C8" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="B9" t="s">
-        <v>228</v>
+        <v>209</v>
       </c>
       <c r="C9" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="B10" t="s">
-        <v>230</v>
+        <v>209</v>
       </c>
       <c r="C10" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="B11" t="s">
-        <v>232</v>
+        <v>209</v>
       </c>
       <c r="C11" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="B12" t="s">
-        <v>234</v>
+        <v>209</v>
       </c>
       <c r="C12" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -1428,7 +1409,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <v>4</v>
@@ -1436,7 +1417,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>2.75</v>
@@ -1444,7 +1425,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <v>5</v>
@@ -1452,7 +1433,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5">
         <v>4.25</v>
@@ -1460,7 +1441,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6">
         <v>2.25</v>
@@ -1468,7 +1449,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7">
         <v>4.75</v>
@@ -1476,7 +1457,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -1511,7 +1492,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2">
         <v>1.5</v>
@@ -1519,7 +1500,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1527,7 +1508,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4">
         <v>0.75</v>
@@ -1535,7 +1516,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -1543,7 +1524,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6">
         <v>3.75</v>
@@ -1551,7 +1532,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7">
         <v>1.5</v>
@@ -1559,7 +1540,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -1567,7 +1548,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9">
         <v>3.75</v>
@@ -1575,7 +1556,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10">
         <v>3.75</v>
@@ -1583,7 +1564,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11">
         <v>7.25</v>
@@ -1591,7 +1572,7 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12">
         <v>3.75</v>
@@ -1599,7 +1580,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B13">
         <v>7.25</v>
@@ -1607,7 +1588,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14">
         <v>1.5</v>
@@ -1615,7 +1596,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -1623,7 +1604,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16">
         <v>3.75</v>
@@ -1631,7 +1612,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B17">
         <v>3</v>
@@ -1639,7 +1620,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B18">
         <v>5.75</v>
@@ -1647,7 +1628,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19">
         <v>3</v>
@@ -1655,7 +1636,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20">
         <v>5.75</v>
@@ -1663,7 +1644,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B21">
         <v>2.75</v>
@@ -1671,7 +1652,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B22">
         <v>3.75</v>
@@ -1679,7 +1660,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B23">
         <v>6</v>
@@ -1714,7 +1695,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -1722,7 +1703,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3">
         <v>2.75</v>
@@ -1730,7 +1711,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4">
         <v>3.25</v>
@@ -1738,7 +1719,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -1746,7 +1727,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6">
         <v>2.5</v>
@@ -1754,7 +1735,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7">
         <v>2.25</v>
@@ -1762,7 +1743,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8">
         <v>2.75</v>
@@ -1770,7 +1751,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9">
         <v>3.5</v>
@@ -1778,7 +1759,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B10">
         <v>3.25</v>
@@ -1786,7 +1767,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B11">
         <v>4.75</v>
@@ -1794,7 +1775,7 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B12">
         <v>2.75</v>
@@ -1802,7 +1783,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B13">
         <v>3.75</v>
@@ -1810,7 +1791,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B14">
         <v>2.75</v>
@@ -1818,7 +1799,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B15">
         <v>3</v>
@@ -1826,7 +1807,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B16">
         <v>3.25</v>
@@ -1834,7 +1815,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B17">
         <v>4</v>
@@ -1842,7 +1823,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B18">
         <v>2.57</v>
@@ -1850,7 +1831,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -1858,7 +1839,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B20">
         <v>3</v>
@@ -1866,7 +1847,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B21">
         <v>3</v>
@@ -1874,7 +1855,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B22">
         <v>4</v>
@@ -1882,7 +1863,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B23">
         <v>2.5</v>
@@ -1890,7 +1871,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B24">
         <v>2.75</v>
@@ -1898,7 +1879,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B25">
         <v>5.5</v>
@@ -1906,7 +1887,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B26">
         <v>4.25</v>
@@ -1914,7 +1895,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B27">
         <v>3</v>
@@ -1922,7 +1903,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B28">
         <v>3</v>
@@ -1930,7 +1911,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B29">
         <v>2.5</v>
@@ -1938,7 +1919,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B30">
         <v>3</v>
@@ -1946,7 +1927,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B31">
         <v>3.25</v>
@@ -1954,7 +1935,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B32">
         <v>2.75</v>
@@ -1962,7 +1943,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B33">
         <v>3</v>
@@ -1970,7 +1951,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B34">
         <v>3</v>
@@ -1978,7 +1959,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B35">
         <v>2.75</v>
@@ -1986,7 +1967,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B36">
         <v>4</v>
@@ -1994,7 +1975,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B37">
         <v>3</v>
@@ -2002,7 +1983,7 @@
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B38">
         <v>3.25</v>
@@ -2010,7 +1991,7 @@
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B39">
         <v>2.75</v>
@@ -2018,7 +1999,7 @@
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B40">
         <v>2.5</v>
@@ -2026,7 +2007,7 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B41">
         <v>2.5</v>
@@ -2034,7 +2015,7 @@
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B42">
         <v>3</v>
@@ -2042,7 +2023,7 @@
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B43">
         <v>5.5</v>
@@ -2050,7 +2031,7 @@
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B44">
         <v>2.75</v>
@@ -2058,7 +2039,7 @@
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B45">
         <v>2.75</v>
@@ -2066,7 +2047,7 @@
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B46">
         <v>2.75</v>
@@ -2074,7 +2055,7 @@
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B47">
         <v>3.25</v>
@@ -2082,7 +2063,7 @@
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B48">
         <v>3.75</v>
@@ -2090,7 +2071,7 @@
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B49">
         <v>2.75</v>
@@ -2098,7 +2079,7 @@
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B50">
         <v>2.75</v>
@@ -2106,7 +2087,7 @@
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B51">
         <v>3</v>
@@ -2114,7 +2095,7 @@
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B52">
         <v>2.75</v>
@@ -2122,7 +2103,7 @@
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B53">
         <v>3.5</v>
@@ -2130,7 +2111,7 @@
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B54">
         <v>2.75</v>
@@ -2138,7 +2119,7 @@
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B55">
         <v>2.75</v>
@@ -2146,7 +2127,7 @@
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B56">
         <v>3.75</v>
@@ -2154,7 +2135,7 @@
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B57">
         <v>3.25</v>
@@ -2162,7 +2143,7 @@
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B58">
         <v>3.25</v>
@@ -2170,7 +2151,7 @@
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B59">
         <v>2.5</v>
@@ -2178,7 +2159,7 @@
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B60">
         <v>3</v>
@@ -2186,7 +2167,7 @@
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B61">
         <v>2.75</v>
@@ -2194,7 +2175,7 @@
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B62">
         <v>3</v>
@@ -2207,7 +2188,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2229,7 +2210,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B2">
         <v>4</v>
@@ -2237,7 +2218,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B3">
         <v>2.75</v>
@@ -2245,7 +2226,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B4">
         <v>3.25</v>
@@ -2253,7 +2234,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B5">
         <v>3.5</v>
@@ -2261,7 +2242,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B6">
         <v>4.75</v>
@@ -2269,7 +2250,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -2277,7 +2258,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B8">
         <v>8.25</v>
@@ -2285,7 +2266,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -2293,25 +2274,17 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B10">
-        <v>9.25</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B11">
-        <v>4.75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>112</v>
-      </c>
-      <c r="B12">
         <v>3.5</v>
       </c>
     </row>
@@ -2344,7 +2317,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2352,7 +2325,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2360,7 +2333,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2368,7 +2341,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B5">
         <v>0.75</v>
@@ -2376,7 +2349,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -2384,7 +2357,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -2392,7 +2365,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -2400,7 +2373,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B9">
         <v>0.75</v>
@@ -2408,7 +2381,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -2416,7 +2389,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B11">
         <v>3</v>
@@ -2424,7 +2397,7 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B12">
         <v>0.75</v>
@@ -2432,7 +2405,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -2440,7 +2413,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B14">
         <v>3</v>
@@ -2448,7 +2421,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -2456,7 +2429,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -2464,7 +2437,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -2472,7 +2445,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -2480,7 +2453,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -2488,7 +2461,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -2496,7 +2469,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B21">
         <v>0.75</v>
@@ -2504,7 +2477,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -2512,7 +2485,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B23">
         <v>3</v>
@@ -2520,7 +2493,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -2528,7 +2501,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -2536,7 +2509,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -2544,7 +2517,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B27">
         <v>2.25</v>
@@ -2552,7 +2525,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B28">
         <v>0.75</v>
@@ -2560,7 +2533,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -2568,7 +2541,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B30">
         <v>3</v>
@@ -2576,7 +2549,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B31">
         <v>0.75</v>
@@ -2584,7 +2557,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -2592,7 +2565,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B33">
         <v>3</v>
@@ -2600,7 +2573,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B34">
         <v>0.75</v>
@@ -2635,7 +2608,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B2">
         <v>5.66</v>
@@ -2643,18 +2616,18 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B3">
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B4">
         <v>5</v>
@@ -2662,7 +2635,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -2670,7 +2643,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -2678,7 +2651,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B7">
         <v>2.75</v>
@@ -2686,7 +2659,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B8">
         <v>4.5</v>
@@ -2694,7 +2667,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B9">
         <v>4</v>
@@ -2702,7 +2675,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B10">
         <v>5</v>
@@ -2710,7 +2683,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B11">
         <v>6</v>
@@ -2718,7 +2691,7 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B12">
         <v>4.5</v>
@@ -2726,7 +2699,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B13">
         <v>5</v>
@@ -2734,7 +2707,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B14">
         <v>1.5</v>
@@ -2742,7 +2715,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B15">
         <v>3</v>
@@ -2750,7 +2723,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B16">
         <v>3</v>
@@ -2758,7 +2731,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B17">
         <v>3</v>
@@ -2766,7 +2739,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B18">
         <v>3</v>
@@ -2774,7 +2747,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -2782,7 +2755,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B20">
         <v>3</v>
@@ -2790,7 +2763,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B21">
         <v>2.5</v>
@@ -2798,7 +2771,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -2806,7 +2779,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -2814,7 +2787,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B24">
         <v>2.5</v>
@@ -2822,7 +2795,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B25">
         <v>2.5</v>
@@ -2830,7 +2803,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B26">
         <v>6</v>
@@ -2838,7 +2811,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B27">
         <v>4.5</v>
@@ -2846,7 +2819,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B28">
         <v>6</v>
@@ -2854,7 +2827,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B29">
         <v>4.5</v>
@@ -2862,7 +2835,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B30">
         <v>3.5</v>
@@ -2870,7 +2843,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B31">
         <v>3.5</v>
@@ -2878,7 +2851,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B32">
         <v>3.5</v>
@@ -2886,7 +2859,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B33">
         <v>6</v>
@@ -2894,7 +2867,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B34">
         <v>3</v>
@@ -2902,7 +2875,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B35">
         <v>5</v>
@@ -2910,7 +2883,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B36">
         <v>4</v>
@@ -2918,7 +2891,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B37">
         <v>0.5</v>
@@ -2953,7 +2926,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B2">
         <v>0.75</v>
@@ -2961,7 +2934,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B3">
         <v>0.25</v>
@@ -2969,7 +2942,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B4">
         <v>0.5</v>
@@ -2977,7 +2950,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2985,7 +2958,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B6">
         <v>0.75</v>
@@ -2993,7 +2966,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3001,7 +2974,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3009,7 +2982,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B9">
         <v>0.75</v>
@@ -3017,7 +2990,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B10">
         <v>1.2</v>
@@ -3025,7 +2998,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B11">
         <v>1.75</v>
@@ -3033,7 +3006,7 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B12">
         <v>0.5</v>
@@ -3041,7 +3014,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B13">
         <v>1.25</v>
@@ -3049,7 +3022,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B14">
         <v>1.5</v>
@@ -3057,7 +3030,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -3065,7 +3038,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B16">
         <v>0.5</v>

</xml_diff>